<commit_message>
added command in loaddata.py
</commit_message>
<xml_diff>
--- a/data/data content .xlsx
+++ b/data/data content .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USA 2020 summer\Machine Learning\Price Prediction Project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\USA 2020 summer\Machine Learning\ds_oil_price_proj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>file name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,16 +72,6 @@
   </si>
   <si>
     <t>https://finance.yahoo.com/quote/%5EGSPC/history?p=%5EGSPC</t>
-  </si>
-  <si>
-    <t>RCLC1d</t>
-  </si>
-  <si>
-    <t>Crude Oil Contract Price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.eia.gov/dnav/pet/hist/RCLC1D.htm</t>
   </si>
   <si>
     <t>WTI Crude Oil Price</t>
@@ -534,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -604,24 +594,24 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -629,10 +619,10 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -640,54 +630,54 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,32 +696,21 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -752,9 +731,8 @@
     <hyperlink ref="C14" r:id="rId13"/>
     <hyperlink ref="C15" r:id="rId14"/>
     <hyperlink ref="C16" r:id="rId15"/>
-    <hyperlink ref="C17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>